<commit_message>
Added Info / Data Flowsensor
</commit_message>
<xml_diff>
--- a/otherinfos/Kalibration/Flusssensor.xlsx
+++ b/otherinfos/Kalibration/Flusssensor.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26924"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{640DF92D-6B73-41E4-96A0-72BDA10BE40B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93C31C29-B97E-4F6D-887C-50C6E8F7C5B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="-135" windowWidth="16440" windowHeight="28440" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Infos" sheetId="10" r:id="rId1"/>
@@ -790,9 +790,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -800,6 +797,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6846,8 +6846,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2AD065A9-0D6C-4C70-9F4A-B063B8DA0137}">
   <dimension ref="B1:L17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="71" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6955,6 +6955,9 @@
       <c r="D4">
         <f>B4/C4</f>
         <v>0.1779359430604982</v>
+      </c>
+      <c r="E4">
+        <v>4256</v>
       </c>
       <c r="F4">
         <v>9.9</v>
@@ -7366,17 +7369,17 @@
   <sheetData>
     <row r="1" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="66" t="s">
+      <c r="B2" s="65" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
-      <c r="F2" s="67"/>
-      <c r="G2" s="67"/>
-      <c r="H2" s="67"/>
-      <c r="I2" s="67"/>
-      <c r="J2" s="68"/>
+      <c r="C2" s="66"/>
+      <c r="D2" s="66"/>
+      <c r="E2" s="66"/>
+      <c r="F2" s="66"/>
+      <c r="G2" s="66"/>
+      <c r="H2" s="66"/>
+      <c r="I2" s="66"/>
+      <c r="J2" s="67"/>
       <c r="S2" t="s">
         <v>26</v>
       </c>
@@ -7615,20 +7618,20 @@
       <c r="I9" s="18"/>
     </row>
     <row r="10" spans="2:27" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="66" t="s">
+      <c r="B10" s="65" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="67"/>
-      <c r="D10" s="67"/>
-      <c r="E10" s="67"/>
-      <c r="F10" s="67"/>
-      <c r="G10" s="67"/>
-      <c r="H10" s="67"/>
-      <c r="I10" s="67"/>
-      <c r="J10" s="68"/>
-      <c r="Y10" s="65"/>
-      <c r="Z10" s="65"/>
-      <c r="AA10" s="65"/>
+      <c r="C10" s="66"/>
+      <c r="D10" s="66"/>
+      <c r="E10" s="66"/>
+      <c r="F10" s="66"/>
+      <c r="G10" s="66"/>
+      <c r="H10" s="66"/>
+      <c r="I10" s="66"/>
+      <c r="J10" s="67"/>
+      <c r="Y10" s="68"/>
+      <c r="Z10" s="68"/>
+      <c r="AA10" s="68"/>
     </row>
     <row r="11" spans="2:27" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="55" t="s">
@@ -8017,17 +8020,17 @@
       <c r="L25" s="2"/>
     </row>
     <row r="26" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B26" s="66" t="s">
+      <c r="B26" s="65" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="68"/>
+      <c r="C26" s="66"/>
+      <c r="D26" s="66"/>
+      <c r="E26" s="66"/>
+      <c r="F26" s="66"/>
+      <c r="G26" s="66"/>
+      <c r="H26" s="66"/>
+      <c r="I26" s="66"/>
+      <c r="J26" s="67"/>
       <c r="L26" s="2"/>
     </row>
     <row r="27" spans="2:15" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -8433,6 +8436,17 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0c8a948-a8a2-431d-a436-e17f069363af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="6b745cbd-a34e-432a-9900-41e3803aa2e9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
@@ -8441,7 +8455,7 @@
 </FormTemplates>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FD8BE65C2F837343AC2660C8B0889EAE" ma:contentTypeVersion="14" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="b7eb9a75dd4706810b4c69081d8d48fe">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="c0c8a948-a8a2-431d-a436-e17f069363af" xmlns:ns3="6b745cbd-a34e-432a-9900-41e3803aa2e9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="f5420ca96eed7fa2cb1a1994b234afa6" ns2:_="" ns3:_="">
     <xsd:import namespace="c0c8a948-a8a2-431d-a436-e17f069363af"/>
@@ -8672,18 +8686,24 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="c0c8a948-a8a2-431d-a436-e17f069363af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="6b745cbd-a34e-432a-9900-41e3803aa2e9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9C1C43-49EE-494C-B635-B785FB629686}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="6b745cbd-a34e-432a-9900-41e3803aa2e9"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="c0c8a948-a8a2-431d-a436-e17f069363af"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E33CB14B-EEEA-4E1E-B623-D870A775B6DB}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
@@ -8691,7 +8711,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A5FF9E8C-A979-49D8-B0D6-7BF035D44D87}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -8708,21 +8728,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{AF9C1C43-49EE-494C-B635-B785FB629686}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="6b745cbd-a34e-432a-9900-41e3803aa2e9"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="c0c8a948-a8a2-431d-a436-e17f069363af"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>